<commit_message>
shape sprites! restructuring non-code resources
Given my limited art skills no need to supporting anything more advanced for art in the interim :')
</commit_message>
<xml_diff>
--- a/resources/GridSprite.xlsx
+++ b/resources/GridSprite.xlsx
@@ -60,7 +60,693 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="168">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -875,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:I14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1154,52 +1840,698 @@
         <v>14</v>
       </c>
     </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>12</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>12</v>
+      </c>
+      <c r="D22">
+        <v>12</v>
+      </c>
+      <c r="E22">
+        <v>12</v>
+      </c>
+      <c r="F22">
+        <v>12</v>
+      </c>
+      <c r="G22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>12</v>
+      </c>
+      <c r="E23">
+        <v>12</v>
+      </c>
+      <c r="F23">
+        <v>12</v>
+      </c>
+      <c r="G23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>12</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <v>6</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>12</v>
+      </c>
+      <c r="D25">
+        <v>12</v>
+      </c>
+      <c r="E25">
+        <v>12</v>
+      </c>
+      <c r="F25">
+        <v>12</v>
+      </c>
+      <c r="G25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>12</v>
+      </c>
+      <c r="E26">
+        <v>12</v>
+      </c>
+      <c r="F26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>4</v>
+      </c>
+      <c r="G30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
+      </c>
+      <c r="G31">
+        <v>4</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <v>4</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>13</v>
+      </c>
+      <c r="C33">
+        <v>13</v>
+      </c>
+      <c r="D33">
+        <v>13</v>
+      </c>
+      <c r="E33">
+        <v>13</v>
+      </c>
+      <c r="F33">
+        <v>13</v>
+      </c>
+      <c r="G33">
+        <v>13</v>
+      </c>
+      <c r="H33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>13</v>
+      </c>
+      <c r="C34">
+        <v>14</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>13</v>
+      </c>
+      <c r="F34">
+        <v>14</v>
+      </c>
+      <c r="G34">
+        <v>3</v>
+      </c>
+      <c r="H34">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>13</v>
+      </c>
+      <c r="C35">
+        <v>14</v>
+      </c>
+      <c r="D35">
+        <v>14</v>
+      </c>
+      <c r="E35">
+        <v>13</v>
+      </c>
+      <c r="F35">
+        <v>14</v>
+      </c>
+      <c r="G35">
+        <v>14</v>
+      </c>
+      <c r="H35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>13</v>
+      </c>
+      <c r="C36">
+        <v>13</v>
+      </c>
+      <c r="D36">
+        <v>13</v>
+      </c>
+      <c r="E36">
+        <v>12</v>
+      </c>
+      <c r="F36">
+        <v>13</v>
+      </c>
+      <c r="G36">
+        <v>13</v>
+      </c>
+      <c r="H36">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>13</v>
+      </c>
+      <c r="C37">
+        <v>13</v>
+      </c>
+      <c r="D37">
+        <v>13</v>
+      </c>
+      <c r="E37">
+        <v>13</v>
+      </c>
+      <c r="F37">
+        <v>13</v>
+      </c>
+      <c r="G37">
+        <v>13</v>
+      </c>
+      <c r="H37">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>13</v>
+      </c>
+      <c r="C38">
+        <v>13</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
+      <c r="F38">
+        <v>5</v>
+      </c>
+      <c r="G38">
+        <v>13</v>
+      </c>
+      <c r="H38">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <v>13</v>
+      </c>
+      <c r="D39">
+        <v>13</v>
+      </c>
+      <c r="E39">
+        <v>13</v>
+      </c>
+      <c r="F39">
+        <v>13</v>
+      </c>
+      <c r="G39">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A21:XFD1048576 M17:XFD20 A1:XFD16 A17:J20">
-    <cfRule type="cellIs" dxfId="69" priority="99" operator="equal">
+  <conditionalFormatting sqref="M17:XFD20 A1:XFD16 A17:J20 A21:XFD29 A40:XFD1048576 A30:E36 G30:XFD36 A37:A38 I37:XFD38 A39:B39 H39:XFD39">
+    <cfRule type="cellIs" dxfId="167" priority="197" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="198" operator="equal">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="199" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="200" operator="equal">
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="201" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="202" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="203" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="204" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="205" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="206" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="207" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="208" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="209" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="210" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17:L17">
+    <cfRule type="cellIs" dxfId="153" priority="141" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="152" priority="142" operator="equal">
+      <formula>12</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="151" priority="143" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="144" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="149" priority="145" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="148" priority="146" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="147" priority="147" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="146" priority="148" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="145" priority="149" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="144" priority="150" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="143" priority="151" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="142" priority="152" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="141" priority="153" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="140" priority="154" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18:L18">
+    <cfRule type="cellIs" dxfId="139" priority="127" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="138" priority="128" operator="equal">
+      <formula>12</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="137" priority="129" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="136" priority="130" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="135" priority="131" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="132" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="133" priority="133" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="132" priority="134" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="131" priority="135" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="136" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="129" priority="137" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="138" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="127" priority="139" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="140" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19:L19">
+    <cfRule type="cellIs" dxfId="125" priority="113" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="124" priority="114" operator="equal">
+      <formula>12</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="123" priority="115" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="116" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="121" priority="117" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="120" priority="118" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="119" priority="119" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="120" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="117" priority="121" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="122" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="115" priority="123" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="124" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="125" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="126" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K20:L20">
+    <cfRule type="cellIs" dxfId="111" priority="99" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="110" priority="100" operator="equal">
+      <formula>12</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="109" priority="101" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="108" priority="102" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="107" priority="103" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="104" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="105" priority="105" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="104" priority="106" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="103" priority="107" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="108" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="109" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="110" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="111" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="112" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F30:F36">
+    <cfRule type="cellIs" dxfId="97" priority="85" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="86" operator="equal">
+      <formula>12</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="87" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="88" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="89" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="90" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="91" priority="91" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="92" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="93" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="94" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="87" priority="95" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="96" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="85" priority="97" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="98" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37:E37 G37:H37">
+    <cfRule type="cellIs" dxfId="83" priority="71" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="72" operator="equal">
+      <formula>12</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="81" priority="73" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="74" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="75" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="76" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="77" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="78" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="79" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="80" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="81" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="82" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="71" priority="83" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="84" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F37">
+    <cfRule type="cellIs" dxfId="69" priority="57" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="58" operator="equal">
+      <formula>12</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="59" operator="equal">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="60" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="65" priority="61" operator="equal">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="62" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="63" operator="equal">
+      <formula>7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="65" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="66" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="67" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="68" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="69" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="70" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38:E38 G38:H38">
     <cfRule type="cellIs" dxfId="55" priority="43" operator="equal">
       <formula>13</formula>
     </cfRule>
@@ -1243,7 +2575,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K18:L18">
+  <conditionalFormatting sqref="F38">
     <cfRule type="cellIs" dxfId="41" priority="29" operator="equal">
       <formula>13</formula>
     </cfRule>
@@ -1287,7 +2619,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K19:L19">
+  <conditionalFormatting sqref="C39:E39 G39">
     <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
       <formula>13</formula>
     </cfRule>
@@ -1331,7 +2663,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K20:L20">
+  <conditionalFormatting sqref="F39">
     <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>13</formula>
     </cfRule>

</xml_diff>

<commit_message>
decoupled shape sprite rendering, updated instructions
Also updated the Colour enums. Which resulted in some odd looking shape sprites for a bit.
</commit_message>
<xml_diff>
--- a/resources/GridSprite.xlsx
+++ b/resources/GridSprite.xlsx
@@ -2,12 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\arcade-rabbit-herder\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12324"/>
   </bookViews>
@@ -60,7 +55,1439 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="168">
+  <dxfs count="370">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA52A2A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD3D3D3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA9A9A9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFADD8E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF90EE90"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE0FFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE97451"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1241,6 +2668,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC99FF"/>
+      <color rgb="FFFF7C80"/>
       <color rgb="FFD373CB"/>
       <color rgb="FFE97451"/>
       <color rgb="FFE0FFFF"/>
@@ -1249,8 +2678,6 @@
       <color rgb="FFA9A9A9"/>
       <color rgb="FFD3D3D3"/>
       <color rgb="FFA52A2A"/>
-      <color rgb="FFFF00FF"/>
-      <color rgb="FF00FFFF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1561,10 +2988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:I39"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1572,7 +2999,7 @@
     <col min="1" max="26" width="3.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1615,113 +3042,116 @@
       <c r="N1">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>13</v>
       </c>
       <c r="D6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G6">
         <v>13</v>
       </c>
       <c r="H6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B7">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>13</v>
       </c>
       <c r="D7">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F7">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G7">
         <v>13</v>
       </c>
       <c r="H7">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B8">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>13</v>
       </c>
       <c r="D8">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F8">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G8">
         <v>13</v>
       </c>
       <c r="H8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H9">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -1742,18 +3172,18 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I10">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -1762,7 +3192,7 @@
         <v>3</v>
       </c>
       <c r="E11">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F11">
         <v>3</v>
@@ -1771,47 +3201,47 @@
         <v>3</v>
       </c>
       <c r="H11">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I11">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I12">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13">
         <v>8</v>
@@ -1823,21 +3253,21 @@
         <v>8</v>
       </c>
       <c r="G13">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H13">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D14">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E14">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F14">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
@@ -2023,7 +3453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>13</v>
       </c>
@@ -2046,12 +3476,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>13</v>
       </c>
       <c r="C34">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D34">
         <v>3</v>
@@ -2060,7 +3490,7 @@
         <v>13</v>
       </c>
       <c r="F34">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G34">
         <v>3</v>
@@ -2069,30 +3499,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>13</v>
       </c>
       <c r="C35">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D35">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E35">
         <v>13</v>
       </c>
       <c r="F35">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G35">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H35">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>13</v>
       </c>
@@ -2115,7 +3545,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>13</v>
       </c>
@@ -2138,7 +3568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>13</v>
       </c>
@@ -2161,7 +3591,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C39">
         <v>13</v>
       </c>
@@ -2178,532 +3608,255 @@
         <v>13</v>
       </c>
     </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E45">
+        <v>10</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <v>10</v>
+      </c>
+      <c r="D46">
+        <v>10</v>
+      </c>
+      <c r="E46">
+        <v>10</v>
+      </c>
+      <c r="F46">
+        <v>10</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>10</v>
+      </c>
+      <c r="E47">
+        <v>10</v>
+      </c>
+      <c r="F47">
+        <v>10</v>
+      </c>
+      <c r="G47">
+        <v>10</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>10</v>
+      </c>
+      <c r="F48">
+        <v>10</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>7</v>
+      </c>
+      <c r="C51">
+        <v>8</v>
+      </c>
+      <c r="D51">
+        <v>8</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>7</v>
+      </c>
+      <c r="C52">
+        <v>7</v>
+      </c>
+      <c r="D52">
+        <v>8</v>
+      </c>
+      <c r="E52">
+        <v>8</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>7</v>
+      </c>
+      <c r="D53">
+        <v>7</v>
+      </c>
+      <c r="E53">
+        <v>8</v>
+      </c>
+      <c r="F53">
+        <v>8</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="M17:XFD20 A1:XFD16 A17:J20 A21:XFD29 A40:XFD1048576 A30:E36 G30:XFD36 A37:A38 I37:XFD38 A39:B39 H39:XFD39">
-    <cfRule type="cellIs" dxfId="167" priority="197" operator="equal">
+  <conditionalFormatting sqref="A1:O1048576">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="equal">
+      <formula>16</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+      <formula>15</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+      <formula>14</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="145" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="146" operator="equal">
       <formula>12</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="165" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="147" operator="equal">
       <formula>11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="200" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="148" operator="equal">
       <formula>10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="149" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="202" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="150" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="203" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="151" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="152" operator="equal">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="159" priority="205" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="153" operator="equal">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="206" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="154" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="157" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="155" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="156" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="209" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="157" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="210" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K17:L17">
-    <cfRule type="cellIs" dxfId="153" priority="141" operator="equal">
-      <formula>13</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="142" operator="equal">
-      <formula>12</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="143" operator="equal">
-      <formula>11</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="144" operator="equal">
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="145" operator="equal">
-      <formula>9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="146" operator="equal">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="147" operator="equal">
-      <formula>7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="148" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="149" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="150" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="151" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="152" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="153" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="154" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18:L18">
-    <cfRule type="cellIs" dxfId="139" priority="127" operator="equal">
-      <formula>13</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="128" operator="equal">
-      <formula>12</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="129" operator="equal">
-      <formula>11</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="130" operator="equal">
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="131" operator="equal">
-      <formula>9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="132" operator="equal">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="133" operator="equal">
-      <formula>7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="134" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="135" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="136" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="137" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="138" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="139" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="140" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K19:L19">
-    <cfRule type="cellIs" dxfId="125" priority="113" operator="equal">
-      <formula>13</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="114" operator="equal">
-      <formula>12</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="115" operator="equal">
-      <formula>11</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="116" operator="equal">
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="117" operator="equal">
-      <formula>9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="118" operator="equal">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="119" operator="equal">
-      <formula>7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="120" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="121" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="122" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="123" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="124" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="125" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="126" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K20:L20">
-    <cfRule type="cellIs" dxfId="111" priority="99" operator="equal">
-      <formula>13</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="100" operator="equal">
-      <formula>12</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="101" operator="equal">
-      <formula>11</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="102" operator="equal">
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="103" operator="equal">
-      <formula>9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="104" operator="equal">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="105" operator="equal">
-      <formula>7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="106" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="107" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="108" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="109" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="110" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="111" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="112" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F30:F36">
-    <cfRule type="cellIs" dxfId="97" priority="85" operator="equal">
-      <formula>13</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="86" operator="equal">
-      <formula>12</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="87" operator="equal">
-      <formula>11</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="88" operator="equal">
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="89" operator="equal">
-      <formula>9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="90" operator="equal">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="91" operator="equal">
-      <formula>7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="92" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="93" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="94" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="95" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="96" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="97" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="98" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B37:E37 G37:H37">
-    <cfRule type="cellIs" dxfId="83" priority="71" operator="equal">
-      <formula>13</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="72" operator="equal">
-      <formula>12</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="73" operator="equal">
-      <formula>11</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="74" operator="equal">
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="75" operator="equal">
-      <formula>9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="76" operator="equal">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="77" operator="equal">
-      <formula>7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="78" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="79" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="80" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="81" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="82" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="83" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="84" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F37">
-    <cfRule type="cellIs" dxfId="69" priority="57" operator="equal">
-      <formula>13</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="58" operator="equal">
-      <formula>12</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="59" operator="equal">
-      <formula>11</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="60" operator="equal">
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="61" operator="equal">
-      <formula>9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="62" operator="equal">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="63" operator="equal">
-      <formula>7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="65" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="66" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="67" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="68" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="69" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="70" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B38:E38 G38:H38">
-    <cfRule type="cellIs" dxfId="55" priority="43" operator="equal">
-      <formula>13</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="44" operator="equal">
-      <formula>12</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="45" operator="equal">
-      <formula>11</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="46" operator="equal">
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="47" operator="equal">
-      <formula>9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="48" operator="equal">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
-      <formula>7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="51" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="52" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="53" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="54" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="55" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="56" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F38">
-    <cfRule type="cellIs" dxfId="41" priority="29" operator="equal">
-      <formula>13</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="30" operator="equal">
-      <formula>12</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="31" operator="equal">
-      <formula>11</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="32" operator="equal">
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="33" operator="equal">
-      <formula>9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
-      <formula>7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="38" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="39" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="40" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="41" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="42" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C39:E39 G39">
-    <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
-      <formula>13</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="16" operator="equal">
-      <formula>12</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="17" operator="equal">
-      <formula>11</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="18" operator="equal">
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
-      <formula>9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
-      <formula>7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="27" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="28" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F39">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
-      <formula>13</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
-      <formula>12</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
-      <formula>11</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
-      <formula>9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
-      <formula>8</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
-      <formula>7</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>6</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
-      <formula>3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="12" operator="equal">
-      <formula>2</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="13" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="158" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>